<commit_message>
commit 19 nov 2018
</commit_message>
<xml_diff>
--- a/src/main/java/com/autopilot/datafiles/TestData.xlsx
+++ b/src/main/java/com/autopilot/datafiles/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A6E0FE-E3E1-4E35-A8AE-8EC5D54C2081}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AB69C4-B443-442B-AA01-4317D44CC504}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -599,7 +599,7 @@
   <dimension ref="A1:BA125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>